<commit_message>
Added instructions for how to create the dataset to feed into linkage()
</commit_message>
<xml_diff>
--- a/data/Kiosk User Patterns Variable List.xlsx
+++ b/data/Kiosk User Patterns Variable List.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\kiosk_user_patterns\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77CF3C1-C4A8-48BF-9FB8-DCF68304A8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9109224B-D250-487B-A1C3-566BB444AF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-13110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-13110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="153">
   <si>
     <t>high_blood_pressure_diagnosis_no</t>
   </si>
@@ -570,6 +571,39 @@
   </si>
   <si>
     <t>Based on your age and gender, have you received the following preventive health screenings? : None of these</t>
+  </si>
+  <si>
+    <t>pseudo_member_id</t>
+  </si>
+  <si>
+    <t>session_id_mask</t>
+  </si>
+  <si>
+    <t>height_inches</t>
+  </si>
+  <si>
+    <t>weight_lbs</t>
+  </si>
+  <si>
+    <t>bp_systolic</t>
+  </si>
+  <si>
+    <t>bmi</t>
+  </si>
+  <si>
+    <t>dasda</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>swdfsf</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -906,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
@@ -2062,4 +2096,142 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F99CE-2F52-49D2-A908-E5E168729789}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2">
+        <v>128</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>140</v>
+      </c>
+      <c r="F2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>